<commit_message>
[card] updated cardpop16 data to have x2 values
</commit_message>
<xml_diff>
--- a/card/data/xlsx/cardpop16.xlsx
+++ b/card/data/xlsx/cardpop16.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WRH\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="11660" yWindow="3140" windowWidth="35300" windowHeight="24220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="82">
   <si>
     <t>Graveyard</t>
   </si>
@@ -208,9 +206,6 @@
   </si>
   <si>
     <t>Furnace</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <t>|</t>
@@ -280,10 +275,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,13 +317,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,7 +386,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,7 +421,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,7 +598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,62 +606,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR53"/>
+  <dimension ref="A1:AR101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE42" sqref="AE42"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52:XFD101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.5" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="11" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -777,7 +792,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -806,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -835,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -864,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -893,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -922,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -951,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -980,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1009,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1038,7 +1053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1067,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1096,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1125,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1154,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1183,7 +1198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1212,7 +1227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1241,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1270,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1299,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38">
       <c r="A20">
         <v>9</v>
       </c>
@@ -1328,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1357,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1386,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38">
       <c r="A23">
         <v>12</v>
       </c>
@@ -1415,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38">
       <c r="A24">
         <v>13</v>
       </c>
@@ -1444,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38">
       <c r="A25">
         <v>14</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38">
       <c r="A26">
         <v>15</v>
       </c>
@@ -1502,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38">
       <c r="A27">
         <v>16</v>
       </c>
@@ -1531,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38">
       <c r="A28">
         <v>17</v>
       </c>
@@ -1560,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38">
       <c r="A29">
         <v>18</v>
       </c>
@@ -1589,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38">
       <c r="A30">
         <v>19</v>
       </c>
@@ -1618,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38">
       <c r="A31">
         <v>20</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38">
       <c r="A32">
         <v>21</v>
       </c>
@@ -1676,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44">
       <c r="A33">
         <v>22</v>
       </c>
@@ -1705,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44">
       <c r="A34">
         <v>23</v>
       </c>
@@ -1734,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44">
       <c r="A35">
         <v>24</v>
       </c>
@@ -1763,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44">
       <c r="A36">
         <v>25</v>
       </c>
@@ -1792,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44">
       <c r="A37">
         <v>26</v>
       </c>
@@ -1821,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44">
       <c r="A38">
         <v>27</v>
       </c>
@@ -1850,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44">
       <c r="A39">
         <v>28</v>
       </c>
@@ -1879,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44">
       <c r="A40">
         <v>29</v>
       </c>
@@ -1908,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44">
       <c r="A41">
         <v>30</v>
       </c>
@@ -1937,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44">
       <c r="A42">
         <v>31</v>
       </c>
@@ -1966,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44">
       <c r="A43">
         <v>32</v>
       </c>
@@ -1995,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44">
       <c r="A44">
         <v>33</v>
       </c>
@@ -2024,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44">
       <c r="A45">
         <v>34</v>
       </c>
@@ -2053,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44">
       <c r="A46">
         <v>35</v>
       </c>
@@ -2082,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44">
       <c r="A47">
         <v>36</v>
       </c>
@@ -2111,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44">
       <c r="A48">
         <v>37</v>
       </c>
@@ -2140,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32">
       <c r="A49">
         <v>38</v>
       </c>
@@ -2169,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32">
       <c r="A50">
         <v>39</v>
       </c>
@@ -2198,7 +2213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32">
       <c r="A51">
         <v>40</v>
       </c>
@@ -2227,316 +2242,1464 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="B52">
-        <f>SUM(B2:B51)</f>
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="R56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="P57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>1</v>
+      </c>
+      <c r="V57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32">
+      <c r="A59" t="s">
         <v>28</v>
       </c>
-      <c r="C52">
-        <f t="shared" ref="C52:AR52" si="0">SUM(C2:C51)</f>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="U59">
+        <v>1</v>
+      </c>
+      <c r="W59">
+        <v>1</v>
+      </c>
+      <c r="X59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Y62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:32">
+      <c r="A63" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="S63">
+        <v>1</v>
+      </c>
+      <c r="U63">
+        <v>1</v>
+      </c>
+      <c r="W63">
+        <v>1</v>
+      </c>
+      <c r="X63">
+        <v>1</v>
+      </c>
+      <c r="Z63">
+        <v>1</v>
+      </c>
+      <c r="AA63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:32">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <v>1</v>
+      </c>
+      <c r="T64">
+        <v>1</v>
+      </c>
+      <c r="U64">
+        <v>1</v>
+      </c>
+      <c r="V64">
+        <v>1</v>
+      </c>
+      <c r="AB64">
+        <v>1</v>
+      </c>
+      <c r="AC64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="O65">
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <v>1</v>
+      </c>
+      <c r="Y65">
+        <v>1</v>
+      </c>
+      <c r="AC65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <v>1</v>
+      </c>
+      <c r="X66">
+        <v>1</v>
+      </c>
+      <c r="AB66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:35">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>1</v>
+      </c>
+      <c r="Q67">
+        <v>1</v>
+      </c>
+      <c r="U67">
+        <v>1</v>
+      </c>
+      <c r="V67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:35">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>1</v>
+      </c>
+      <c r="P68">
+        <v>1</v>
+      </c>
+      <c r="Y68">
+        <v>1</v>
+      </c>
+      <c r="AD68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <v>1</v>
+      </c>
+      <c r="P69">
+        <v>1</v>
+      </c>
+      <c r="V69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:35">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="N70">
+        <v>1</v>
+      </c>
+      <c r="V70">
+        <v>1</v>
+      </c>
+      <c r="Y70">
+        <v>1</v>
+      </c>
+      <c r="AE70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:35">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:35">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="M72">
+        <v>1</v>
+      </c>
+      <c r="P72">
+        <v>1</v>
+      </c>
+      <c r="S72">
+        <v>1</v>
+      </c>
+      <c r="T72">
+        <v>1</v>
+      </c>
+      <c r="U72">
+        <v>1</v>
+      </c>
+      <c r="V72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:35">
+      <c r="A73">
+        <v>12</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <v>1</v>
+      </c>
+      <c r="V73">
+        <v>1</v>
+      </c>
+      <c r="AA73">
+        <v>1</v>
+      </c>
+      <c r="AF73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:35">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:35">
+      <c r="A75">
+        <v>14</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="Y75">
+        <v>1</v>
+      </c>
+      <c r="AE75">
+        <v>1</v>
+      </c>
+      <c r="AG75">
+        <v>1</v>
+      </c>
+      <c r="AH75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:35">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="Q76">
+        <v>1</v>
+      </c>
+      <c r="V76">
+        <v>1</v>
+      </c>
+      <c r="AH76">
+        <v>1</v>
+      </c>
+      <c r="AI76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35">
+      <c r="A77">
+        <v>16</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>1</v>
+      </c>
+      <c r="S77">
+        <v>1</v>
+      </c>
+      <c r="U77">
+        <v>1</v>
+      </c>
+      <c r="V77">
+        <v>1</v>
+      </c>
+      <c r="W77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35">
+      <c r="A78">
+        <v>17</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+      <c r="S78">
+        <v>1</v>
+      </c>
+      <c r="V78">
+        <v>1</v>
+      </c>
+      <c r="W78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35">
+      <c r="A79">
+        <v>18</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="Q79">
+        <v>1</v>
+      </c>
+      <c r="AH79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35">
+      <c r="A80">
+        <v>19</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <v>1</v>
+      </c>
+      <c r="U80">
+        <v>1</v>
+      </c>
+      <c r="V80">
+        <v>1</v>
+      </c>
+      <c r="AC80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:44">
+      <c r="A81">
+        <v>20</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+      <c r="O81">
+        <v>1</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+      <c r="Y81">
+        <v>1</v>
+      </c>
+      <c r="AJ81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:44">
+      <c r="A82">
+        <v>21</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="S82">
+        <v>1</v>
+      </c>
+      <c r="W82">
+        <v>1</v>
+      </c>
+      <c r="X82">
+        <v>1</v>
+      </c>
+      <c r="AA82">
+        <v>1</v>
+      </c>
+      <c r="AB82">
+        <v>1</v>
+      </c>
+      <c r="AK82">
+        <v>1</v>
+      </c>
+      <c r="AL82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:44">
+      <c r="A83">
+        <v>22</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="AM83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:44">
+      <c r="A84">
+        <v>23</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="AN84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:44">
+      <c r="A85">
+        <v>24</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:44">
+      <c r="A86">
+        <v>25</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="Q86">
+        <v>1</v>
+      </c>
+      <c r="S86">
+        <v>1</v>
+      </c>
+      <c r="T86">
+        <v>1</v>
+      </c>
+      <c r="U86">
+        <v>1</v>
+      </c>
+      <c r="X86">
+        <v>1</v>
+      </c>
+      <c r="AF86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:44">
+      <c r="A87">
+        <v>26</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="M87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:44">
+      <c r="A88">
         <v>27</v>
       </c>
-      <c r="D52">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="0"/>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:44">
+      <c r="A89">
+        <v>28</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="O89">
+        <v>1</v>
+      </c>
+      <c r="Q89">
+        <v>1</v>
+      </c>
+      <c r="R89">
+        <v>1</v>
+      </c>
+      <c r="U89">
+        <v>1</v>
+      </c>
+      <c r="AL89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:44">
+      <c r="A90">
+        <v>29</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>1</v>
+      </c>
+      <c r="Q90">
+        <v>1</v>
+      </c>
+      <c r="U90">
+        <v>1</v>
+      </c>
+      <c r="X90">
+        <v>1</v>
+      </c>
+      <c r="AD90">
+        <v>1</v>
+      </c>
+      <c r="AO90">
+        <v>1</v>
+      </c>
+      <c r="AP90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:44">
+      <c r="A91">
         <v>30</v>
       </c>
-      <c r="H52">
-        <f t="shared" si="0"/>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="R91">
+        <v>1</v>
+      </c>
+      <c r="S91">
+        <v>1</v>
+      </c>
+      <c r="AN91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:44">
+      <c r="A92">
+        <v>31</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>1</v>
+      </c>
+      <c r="U92">
+        <v>1</v>
+      </c>
+      <c r="X92">
+        <v>1</v>
+      </c>
+      <c r="AA92">
+        <v>1</v>
+      </c>
+      <c r="AQ92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:44">
+      <c r="A93">
+        <v>32</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="M93">
+        <v>1</v>
+      </c>
+      <c r="N93">
+        <v>1</v>
+      </c>
+      <c r="Y93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:44">
+      <c r="A94">
+        <v>33</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="S94">
+        <v>1</v>
+      </c>
+      <c r="AB94">
+        <v>1</v>
+      </c>
+      <c r="AJ94">
+        <v>1</v>
+      </c>
+      <c r="AR94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:44">
+      <c r="A95">
         <v>34</v>
       </c>
-      <c r="I52">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M52">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O52">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="P52">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q52">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="R52">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="S52">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="T52">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="U52">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="V52">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="W52">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="X52">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="Y52">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="Z52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AA52">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="AB52">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="AC52">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AD52">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AE52">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AF52">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AG52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AH52">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AI52">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AJ52">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AK52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AL52">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AM52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AN52">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AO52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AP52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AQ52">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AR52">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" t="s">
-        <v>3</v>
-      </c>
-      <c r="G53" t="s">
-        <v>4</v>
-      </c>
-      <c r="H53" t="s">
-        <v>5</v>
-      </c>
-      <c r="I53" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" t="s">
-        <v>8</v>
-      </c>
-      <c r="K53" t="s">
-        <v>9</v>
-      </c>
-      <c r="L53" t="s">
-        <v>10</v>
-      </c>
-      <c r="M53" t="s">
-        <v>15</v>
-      </c>
-      <c r="N53" t="s">
-        <v>0</v>
-      </c>
-      <c r="O53" t="s">
-        <v>17</v>
-      </c>
-      <c r="P53" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>19</v>
-      </c>
-      <c r="R53" t="s">
-        <v>21</v>
-      </c>
-      <c r="S53" t="s">
-        <v>23</v>
-      </c>
-      <c r="T53" t="s">
-        <v>24</v>
-      </c>
-      <c r="U53" t="s">
-        <v>25</v>
-      </c>
-      <c r="V53" t="s">
-        <v>26</v>
-      </c>
-      <c r="W53" t="s">
-        <v>29</v>
-      </c>
-      <c r="X53" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y53" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z53" t="s">
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="O95">
+        <v>1</v>
+      </c>
+      <c r="R95">
+        <v>1</v>
+      </c>
+      <c r="S95">
+        <v>1</v>
+      </c>
+      <c r="V95">
+        <v>1</v>
+      </c>
+      <c r="AA95">
+        <v>1</v>
+      </c>
+      <c r="AQ95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:44">
+      <c r="A96">
+        <v>35</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="AA96">
+        <v>1</v>
+      </c>
+      <c r="AR96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:35">
+      <c r="A97">
         <v>36</v>
       </c>
-      <c r="AA53" t="s">
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:35">
+      <c r="A98">
         <v>37</v>
       </c>
-      <c r="AB53" t="s">
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+      <c r="AB98">
+        <v>1</v>
+      </c>
+      <c r="AD98">
+        <v>1</v>
+      </c>
+      <c r="AI98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:35">
+      <c r="A99">
+        <v>38</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:35">
+      <c r="A100">
         <v>39</v>
       </c>
-      <c r="AC53" t="s">
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="O100">
+        <v>1</v>
+      </c>
+      <c r="P100">
+        <v>1</v>
+      </c>
+      <c r="Q100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:35">
+      <c r="A101">
         <v>40</v>
       </c>
-      <c r="AD53" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE53" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF53" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG53" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH53" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI53" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ53" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK53" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL53" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM53" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN53" t="s">
-        <v>56</v>
-      </c>
-      <c r="AO53" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP53" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ53" t="s">
-        <v>59</v>
-      </c>
-      <c r="AR53" t="s">
-        <v>60</v>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="O101">
+        <v>1</v>
+      </c>
+      <c r="Q101">
+        <v>1</v>
+      </c>
+      <c r="AF101">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2548,1057 +3711,1057 @@
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1">
         <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2">
         <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9">
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <v>-33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <v>-14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13">
         <v>-24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14">
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14">
         <v>-9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17">
         <v>-3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18">
         <v>-11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19">
         <v>-37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21">
         <v>-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22">
         <v>-7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24">
         <v>-18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26">
         <v>-11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27">
         <v>-20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29">
         <v>-11</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30">
         <v>-7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32">
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33">
         <v>-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34">
         <v>-14</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E36">
         <v>-3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E39">
         <v>-9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E41">
         <v>-9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42">
         <v>-12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47">
         <v>-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E49">
         <v>-5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E51">
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E52">
         <v>-3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E54">
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E55">
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E58">
         <v>-10</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E59">
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E60">
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -3609,6 +4772,11 @@
     <sortCondition descending="1" ref="C1:C62"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>